<commit_message>
Added EU LCS Spring 2018 game ids and hashes spreadsheet.
</commit_message>
<xml_diff>
--- a/nalcs_spring2018.xlsx
+++ b/nalcs_spring2018.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="162">
   <si>
     <t>NA LCS Spring Split 2018</t>
   </si>
@@ -524,6 +524,9 @@
   </si>
   <si>
     <t>0e19ce71fe99bf30</t>
+  </si>
+  <si>
+    <t>Region ID</t>
   </si>
 </sst>
 </file>
@@ -935,32 +938,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D145"/>
+  <dimension ref="A1:E145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>126</v>
       </c>
@@ -968,7 +972,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -976,13 +980,16 @@
         <v>32</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
@@ -990,1757 +997,2108 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="5">
         <v>1002440062</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6">
         <v>1002440076</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5">
         <v>1002440084</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5">
         <v>1002440095</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="5">
         <v>1002440106</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5">
         <v>1002440127</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="5">
         <v>1002440132</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="5">
         <v>1002440143</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="5">
         <v>1002440150</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5">
         <v>1002440161</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="5">
         <v>1002440178</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="5">
         <v>1002440188</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="5">
         <v>1002440193</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="5">
         <v>1002440202</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="5">
         <v>1002440210</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="5">
         <v>1002440231</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="5">
         <v>1002440242</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="5">
         <v>1002440256</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="5">
         <v>1002440271</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="E26" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="5">
         <v>1002440282</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="E27" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B29" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="5">
         <v>1002450006</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="E29" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B30" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="5">
         <v>1002450017</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="5">
         <v>1002450029</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="E31" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="5">
         <v>1002450040</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="5">
         <v>1002450050</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="E33" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B35" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="5">
         <v>1002450066</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="5">
         <v>1002450079</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="E36" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="5">
         <v>1002450088</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="5">
         <v>1002450096</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="E38" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="5">
         <v>1002450114</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="E39" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="5">
         <v>1002450127</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="E41" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>3</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="5">
         <v>1002450145</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="E42" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="5">
         <v>1002450156</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="E43" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="5">
         <v>1002450163</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="E44" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="5">
         <v>1002450171</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B47" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="5">
         <v>1002450187</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="E47" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="5">
         <v>1002450191</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="E48" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B49" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="5">
         <v>1002450204</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="E49" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="5">
         <v>1002450212</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="E50" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>9</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C51" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="5">
         <v>1002450220</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="E51" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C53" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="5">
         <v>1002470009</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="E53" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C54" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="5">
         <v>1002470017</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="E54" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C55" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="5">
         <v>1002470023</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="E55" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C56" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="5">
         <v>1002470030</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="E56" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C57" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="5">
         <v>1002470039</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="E57" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B59" t="s">
         <v>4</v>
       </c>
-      <c r="C59" s="5">
+      <c r="C59" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="5">
         <v>1002470050</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="E59" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B60" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="5">
+      <c r="C60" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="5">
         <v>1002470053</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="E60" s="5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B61" t="s">
         <v>25</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C61" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="5">
         <v>1002470057</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="E61" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B62" t="s">
         <v>18</v>
       </c>
-      <c r="C62" s="5">
+      <c r="C62" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="5">
         <v>1002470068</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="E62" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B63" t="s">
         <v>9</v>
       </c>
-      <c r="C63" s="5">
+      <c r="C63" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="5">
         <v>1002470072</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="E63" s="5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B65" t="s">
         <v>25</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C65" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="5">
         <v>1002480123</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="E65" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C66" s="5">
+      <c r="C66" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="5">
         <v>1002480129</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="E66" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B67" t="s">
         <v>15</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C67" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" s="5">
         <v>1002480138</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="E67" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C68" s="5">
+      <c r="C68" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" s="5">
         <v>1002480149</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="E68" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B69" t="s">
         <v>16</v>
       </c>
-      <c r="C69" s="5">
+      <c r="C69" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" s="5">
         <v>1002480157</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="E69" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>9</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C71" s="5">
+      <c r="C71" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="5">
         <v>1002480175</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="E71" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>16</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C72" s="5">
+      <c r="C72" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="5">
         <v>1002480185</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="E72" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C73" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="5">
         <v>1002480198</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="E73" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>18</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C74" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="5">
         <v>1002480206</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="E74" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C75" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="5">
         <v>1002480213</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="E75" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B77" t="s">
         <v>8</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C77" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D77" s="5">
         <v>1002490013</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="E77" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B78" t="s">
         <v>16</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C78" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D78" s="5">
         <v>1002490026</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="E78" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B79" t="s">
         <v>25</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C79" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D79" s="5">
         <v>1002490037</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="E79" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B80" t="s">
         <v>15</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C80" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="5">
         <v>1002490045</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="E80" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B81" t="s">
         <v>9</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C81" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D81" s="5">
         <v>1002490053</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="E81" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B83" t="s">
         <v>3</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C83" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D83" s="5">
         <v>1002490071</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="E83" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C84" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84" s="5">
         <v>1002490078</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="E84" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B85" t="s">
         <v>4</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C85" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D85" s="5">
         <v>1002490088</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="E85" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B86" t="s">
         <v>12</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C86" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="5">
         <v>1002490095</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="E86" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C87" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87" s="5">
         <v>1002490102</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="E87" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B89" t="s">
         <v>15</v>
       </c>
-      <c r="C89" s="5">
+      <c r="C89" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" s="5">
         <v>1002500096</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="E89" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C90" s="5">
+      <c r="C90" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D90" s="5">
         <v>1002500103</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="E90" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>9</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C91" s="5">
+      <c r="C91" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="5">
         <v>1002500110</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="E91" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C92" s="5">
+      <c r="C92" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="5">
         <v>1002500116</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="E92" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C93" s="5">
+      <c r="C93" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" s="5">
         <v>1002500123</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="E93" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>15</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C95" s="5">
+      <c r="C95" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D95" s="5">
         <v>1002500146</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="E95" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B96" t="s">
         <v>12</v>
       </c>
-      <c r="C96" s="5">
+      <c r="C96" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" s="5">
         <v>1002500150</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="E96" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C97" s="5">
+      <c r="C97" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" s="5">
         <v>1002500155</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="E97" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>25</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C98" s="5">
+      <c r="C98" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" s="5">
         <v>1002500163</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="E98" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>9</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C99" s="5">
+      <c r="C99" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" s="5">
         <v>1002500172</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="E99" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C101" s="5">
+      <c r="C101" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" s="5">
         <v>1002510019</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="E101" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>16</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C102" s="5">
+      <c r="C102" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D102" s="5">
         <v>1002510023</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="E102" s="5" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C103" s="5">
+      <c r="C103" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D103" s="5">
         <v>1002510029</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="E103" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>12</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C104" s="5">
+      <c r="C104" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="5">
         <v>1002510037</v>
       </c>
-      <c r="D104" s="5" t="s">
+      <c r="E104" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>18</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C105" s="5">
+      <c r="C105" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D105" s="5">
         <v>1002510046</v>
       </c>
-      <c r="D105" s="5" t="s">
+      <c r="E105" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>25</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C107" s="5">
+      <c r="C107" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" s="5">
         <v>1002510062</v>
       </c>
-      <c r="D107" s="5" t="s">
+      <c r="E107" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>12</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C108" s="5">
+      <c r="C108" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D108" s="5">
         <v>1002510068</v>
       </c>
-      <c r="D108" s="5" t="s">
+      <c r="E108" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>18</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C109" s="5">
+      <c r="C109" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" s="5">
         <v>1002510077</v>
       </c>
-      <c r="D109" s="5" t="s">
+      <c r="E109" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C110" s="5">
+      <c r="C110" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D110" s="5">
         <v>1002510083</v>
       </c>
-      <c r="D110" s="5" t="s">
+      <c r="E110" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C111" s="5">
+      <c r="C111" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" s="5">
         <v>1002510092</v>
       </c>
-      <c r="D111" s="5" t="s">
+      <c r="E111" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B112" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C112" s="12">
+      <c r="C112" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D112" s="12">
         <v>1002510099</v>
       </c>
-      <c r="D112" s="12" t="s">
+      <c r="E112" s="12" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B113" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C113" s="12">
+      <c r="C113" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" s="12">
         <v>1002510106</v>
       </c>
-      <c r="D113" s="12" t="s">
+      <c r="E113" s="12" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B114" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C114" s="12">
+      <c r="C114" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D114" s="12">
         <v>1002510113</v>
       </c>
-      <c r="D114" s="12" t="s">
+      <c r="E114" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B115" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C115" s="12">
+      <c r="C115" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D115" s="12">
         <v>1002510123</v>
       </c>
-      <c r="D115" s="12" t="s">
+      <c r="E115" s="12" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C116" s="12">
+      <c r="C116" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D116" s="12">
         <v>1002510129</v>
       </c>
-      <c r="D116" s="12" t="s">
+      <c r="E116" s="12" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B119" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C119" s="14">
+      <c r="C119" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D119" s="14">
         <v>1002510203</v>
       </c>
-      <c r="D119" s="14" t="s">
+      <c r="E119" s="14" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B120" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C120" s="14">
+      <c r="C120" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D120" s="14">
         <v>1002510212</v>
       </c>
-      <c r="D120" s="14" t="s">
+      <c r="E120" s="14" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B121" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C121" s="14">
+      <c r="C121" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D121" s="14">
         <v>1002510216</v>
       </c>
-      <c r="D121" s="14" t="s">
+      <c r="E121" s="14" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B123" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C123" s="14">
+      <c r="C123" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D123" s="14">
         <v>1002520202</v>
       </c>
-      <c r="D123" s="14" t="s">
+      <c r="E123" s="14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B124" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C124" s="14">
+      <c r="C124" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D124" s="14">
         <v>1002520204</v>
       </c>
-      <c r="D124" s="14" t="s">
+      <c r="E124" s="14" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="15" t="s">
         <v>4</v>
       </c>
       <c r="B125" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C125" s="14">
+      <c r="C125" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D125" s="14">
         <v>1002520205</v>
       </c>
-      <c r="D125" s="14" t="s">
+      <c r="E125" s="14" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B126" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C126" s="14">
+      <c r="C126" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D126" s="14">
         <v>1002520206</v>
       </c>
-      <c r="D126" s="14" t="s">
+      <c r="E126" s="14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B128" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C128" s="14">
+      <c r="C128" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D128" s="14">
         <v>1002520246</v>
       </c>
-      <c r="D128" s="14" t="s">
+      <c r="E128" s="14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B129" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C129" s="14">
+      <c r="C129" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D129" s="14">
         <v>1002520249</v>
       </c>
-      <c r="D129" s="14" t="s">
+      <c r="E129" s="14" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B130" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C130" s="14">
+      <c r="C130" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D130" s="14">
         <v>1002520250</v>
       </c>
-      <c r="D130" s="14" t="s">
+      <c r="E130" s="14" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B131" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C131" s="14">
+      <c r="C131" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D131" s="14">
         <v>1002520251</v>
       </c>
-      <c r="D131" s="14" t="s">
+      <c r="E131" s="14" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B133" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C133" s="14">
+      <c r="C133" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D133" s="14">
         <v>1002520263</v>
       </c>
-      <c r="D133" s="14" t="s">
+      <c r="E133" s="14" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B134" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C134" s="14">
+      <c r="C134" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D134" s="14">
         <v>1002520265</v>
       </c>
-      <c r="D134" s="14" t="s">
+      <c r="E134" s="14" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B135" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C135" s="14">
+      <c r="C135" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D135" s="14">
         <v>1002520266</v>
       </c>
-      <c r="D135" s="14" t="s">
+      <c r="E135" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B136" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C136" s="14">
+      <c r="C136" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D136" s="14">
         <v>1002520267</v>
       </c>
-      <c r="D136" s="16" t="s">
+      <c r="E136" s="16" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B137" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C137" s="14">
+      <c r="C137" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D137" s="14">
         <v>1002520268</v>
       </c>
-      <c r="D137" s="14" t="s">
+      <c r="E137" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B139" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C139" s="14">
+      <c r="C139" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D139" s="14">
         <v>1002530054</v>
       </c>
-      <c r="D139" s="16" t="s">
+      <c r="E139" s="16" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B140" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C140" s="14">
+      <c r="C140" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D140" s="14">
         <v>1002530055</v>
       </c>
-      <c r="D140" s="14" t="s">
+      <c r="E140" s="14" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B141" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C141" s="14">
+      <c r="C141" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D141" s="14">
         <v>1002530058</v>
       </c>
-      <c r="D141" s="14" t="s">
+      <c r="E141" s="14" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B143" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C143" s="14">
+      <c r="C143" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D143" s="14">
         <v>1002530069</v>
       </c>
-      <c r="D143" s="14" t="s">
+      <c r="E143" s="14" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B144" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C144" s="14">
+      <c r="C144" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D144" s="14">
         <v>1002530071</v>
       </c>
-      <c r="D144" s="14" t="s">
+      <c r="E144" s="14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B145" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C145" s="14">
+      <c r="C145" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D145" s="14">
         <v>1002530072</v>
       </c>
-      <c r="D145" s="14" t="s">
+      <c r="E145" s="14" t="s">
         <v>160</v>
       </c>
     </row>

</xml_diff>